<commit_message>
output van verschillende runs opgeslagen
</commit_message>
<xml_diff>
--- a/code/experiments/anneal_results/testrun_gevoeligheid/analyse.xlsx
+++ b/code/experiments/anneal_results/testrun_gevoeligheid/analyse.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gobel\Desktop\Programming\AH\WSV\code\experiments\grid_search_tabu_results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gobel\Desktop\Programming\AH\WSV\code\experiments\anneal_results\testrun_gevoeligheid\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B9124337-B3D8-4685-915C-2261E7AA303D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56C4AA3C-5D87-42A7-B37D-2D00343979AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="new_file" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,20 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">new_file!$A$1:$K$10</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -35,7 +48,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -633,26 +646,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="nl-NL"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:view3D>
@@ -2000,7 +1993,17 @@
               </a:p>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="nl-NL"/>
@@ -2009,7 +2012,17 @@
               </a:p>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="nl-NL"/>
@@ -2034,26 +2047,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="nl-NL"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
@@ -2160,26 +2153,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="nl-NL"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -2249,7 +2222,17 @@
               </a:p>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="nl-NL"/>
@@ -2279,26 +2262,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="nl-NL"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
@@ -5267,16 +5230,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>395287</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>138112</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>528637</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>119062</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>90487</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>23812</xdr:rowOff>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>223837</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5638,7 +5601,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5998,7 +5961,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K10">
+  <autoFilter ref="A1:K10" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K10">
       <sortCondition ref="A1:A10"/>
     </sortState>
@@ -6008,11 +5971,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="I5:V17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V11" sqref="V11"/>
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6493,7 +6456,7 @@
         <v>123.55999999999979</v>
       </c>
       <c r="L17">
-        <f t="shared" ref="L17:U17" si="2">AVERAGE(L7:L16)</f>
+        <f t="shared" ref="L17:T17" si="2">AVERAGE(L7:L16)</f>
         <v>128.94999999999979</v>
       </c>
       <c r="M17">

</xml_diff>